<commit_message>
Few changes in test case 6 and added it to testng.xml suit
</commit_message>
<xml_diff>
--- a/src/test/java/rc25/mFormsAutomation/TestData/UserRegistration.xlsx
+++ b/src/test/java/rc25/mFormsAutomation/TestData/UserRegistration.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -171,10 +171,10 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Donefc.sat.ms@quetaeffseper.net</t>
-  </si>
-  <si>
-    <t>mrsi.loris@Lfrm.ca</t>
+    <t>Donefc.sat.ms@quetbhaeffseper.net</t>
+  </si>
+  <si>
+    <t>mrsi.loris@Lfbnrm.caarrr</t>
   </si>
 </sst>
 </file>
@@ -606,7 +606,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -678,42 +678,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -721,10 +688,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="A1:XFD6"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -873,10 +840,43 @@
         <v>7</v>
       </c>
     </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1"/>
     <hyperlink ref="A6" r:id="rId2"/>
+    <hyperlink ref="A7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>